<commit_message>
Update envio de email
</commit_message>
<xml_diff>
--- a/relatorios_padaria/Vendas_Diarias/Relatorio_de_Vendas_Diarias_29-08-2025.xlsx
+++ b/relatorios_padaria/Vendas_Diarias/Relatorio_de_Vendas_Diarias_29-08-2025.xlsx
@@ -498,7 +498,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>18</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6">
@@ -538,7 +538,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>10000535.5</v>
+        <v>10000657.5</v>
       </c>
     </row>
     <row r="11">
@@ -559,7 +559,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -826,8 +826,58 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Venda Balcão</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>75</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>29/08/2025 23:02:26</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>receita</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Dinheiro</t>
+        </is>
+      </c>
+    </row>
     <row r="12">
-      <c r="A12" s="3" t="inlineStr">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Venda Balcão</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>29/08/2025 23:05:18</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>receita</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Dinheiro</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
         <is>
           <t>Sistema desenvolvido por ROBSON ALVES</t>
         </is>

</xml_diff>